<commit_message>
add total nilai konversi
</commit_message>
<xml_diff>
--- a/storage/app/def.xlsx
+++ b/storage/app/def.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="204">
   <si>
     <t>Timestamp</t>
   </si>
@@ -48,27 +48,15 @@
     <t xml:space="preserve">Proses dari benda padat menjadi uap </t>
   </si>
   <si>
-    <t>Karena terjadi pemuaian pada siang hari, jika pemuaian terjadi maka masih ada tempat. Sehingga rel tidak bengkok.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perubahan penampilan </t>
-  </si>
-  <si>
     <t>Karena adanya rotasi bumi</t>
   </si>
   <si>
-    <t>Perubahan wujud dari padat menjadi gas</t>
-  </si>
-  <si>
     <t>Karena massa jenis kayu lebih kecil daripada air</t>
   </si>
   <si>
     <t>karena saat panas rel kereta memuai</t>
   </si>
   <si>
-    <t>perkembangan biologi pada hewan</t>
-  </si>
-  <si>
     <t xml:space="preserve">karena bumi berotasi </t>
   </si>
   <si>
@@ -81,24 +69,9 @@
     <t>perubahan dari padat ke gas</t>
   </si>
   <si>
-    <t>Karena mencegah pemuaian saat siang hari dan mencegah penyusutan saat malam hari</t>
-  </si>
-  <si>
-    <t>Suatu proses perkembangan pada pertumbuhan sel</t>
-  </si>
-  <si>
-    <t>Karena matahari dan bumi melakukan rotasi maka terjadilah siang dan malam</t>
-  </si>
-  <si>
-    <t>Perubahan wujud padat ke wujud gas</t>
-  </si>
-  <si>
     <t>Karena massa jenis kayu kecil</t>
   </si>
   <si>
-    <t>Agar saat terjadi pemuaian rel tidak bengkok</t>
-  </si>
-  <si>
     <t>Perubahan bentuk fisik</t>
   </si>
   <si>
@@ -114,33 +87,18 @@
     <t>Proses perubahan bentuk pada hewan yang melibatkan perubahan fisik</t>
   </si>
   <si>
-    <t>Karena bumi mengelilingi matahari dan bumi berputar pada porosnya (karena bumi melakukan revolusi &amp; rotasi)</t>
-  </si>
-  <si>
     <t>untuk mengantisipasi terjadinya pemuaian di siang hari</t>
   </si>
   <si>
-    <t>Perkembangan biologi pada hewan</t>
-  </si>
-  <si>
     <t>Adanya rotasi bumi</t>
   </si>
   <si>
     <t>perubahan wujud benda dari gas menjadi benda cair</t>
   </si>
   <si>
-    <t>Perubahan dari telur, ulat, kepompong, kupu-kupu, kasian deh lu *sambil nyanyi. Intinya suatu perubahan dari mahluk hidup untuk lebih sempurna</t>
-  </si>
-  <si>
-    <t>Karena bumi berputar pada porosnya, mengelilingi matahari/sebaliknya</t>
-  </si>
-  <si>
     <t>Proses penguapan pada benda padat yang menjadi uap?</t>
   </si>
   <si>
-    <t xml:space="preserve">Perubahan penampilan/bentuk/struktur biologis dalam masa perkembangan hewan </t>
-  </si>
-  <si>
     <t>Perubahan benda padat menjadi gas</t>
   </si>
   <si>
@@ -162,9 +120,6 @@
     <t>Karena bumi berotasi</t>
   </si>
   <si>
-    <t>Zat padat berubah menjadi gas</t>
-  </si>
-  <si>
     <t>Karena beratnya lebih ringan</t>
   </si>
   <si>
@@ -174,15 +129,9 @@
     <t>karena bumi berotasi</t>
   </si>
   <si>
-    <t>perubahan benda padat menjadi gas</t>
-  </si>
-  <si>
     <t>karena massa kayu lebih ringan daripada air</t>
   </si>
   <si>
-    <t>Perubahan wujud dari padat menjadi gas.</t>
-  </si>
-  <si>
     <t>Karena supaya tidak ada tabrakan</t>
   </si>
   <si>
@@ -201,9 +150,6 @@
     <t>perkembangan bentuk hewan</t>
   </si>
   <si>
-    <t>perubahan dari benda padat menjadi gas</t>
-  </si>
-  <si>
     <t>karena massa jenis kayu kecil</t>
   </si>
   <si>
@@ -213,30 +159,9 @@
     <t>massa jenis kayu lebih ringan daripada massa jenis air</t>
   </si>
   <si>
-    <t>Menghindari pemuaian pada siang hari.</t>
-  </si>
-  <si>
-    <t>Adanya rotasi bumi.</t>
-  </si>
-  <si>
-    <t>Perubahan dari zat padat ke gas.</t>
-  </si>
-  <si>
-    <t>Karena kayu memiliki serat.</t>
-  </si>
-  <si>
     <t xml:space="preserve">mengantisipasi pemuaian pada rel kereta api </t>
   </si>
   <si>
-    <t>perubahan wujud hidup suatu mahluk hidup dari telur, ulat, pupa, hingga kupu-kupu dewasa</t>
-  </si>
-  <si>
-    <t>karena bumi berotasi (berputar pada porosnya), sehingga seolah matahari berpindah dari timur ke barat</t>
-  </si>
-  <si>
-    <t>Proses perubahan dari larva sampai jadi kupu kupu</t>
-  </si>
-  <si>
     <t>Bumi berputar pada porosnya</t>
   </si>
   <si>
@@ -261,12 +186,6 @@
     <t xml:space="preserve">Karena pada siang hari rel besi memuai sehingga perlu tempat untuk jadi panjang </t>
   </si>
   <si>
-    <t>Proses perkembangan pada hewan</t>
-  </si>
-  <si>
-    <t>Perubahan bentuk wujud dari padat menjadi gas</t>
-  </si>
-  <si>
     <t>Gaya apung&gt; Dari gaya gravitasi</t>
   </si>
   <si>
@@ -291,42 +210,18 @@
     <t>Siklus perubahan suatu makhluk hidup di mana fisik pada fase larvanya berbeda dengan fisik pada fase dewasanya</t>
   </si>
   <si>
-    <t>Karena bumi melakukan rotasi sehingga terjadi perubahan siang dan malam</t>
-  </si>
-  <si>
-    <t>Perubahan fase jenis benda dari padat ke uap</t>
-  </si>
-  <si>
     <t>Karena massa jenis kayu lebih kecil daripada massa jenis air</t>
   </si>
   <si>
-    <t>perubahan bentuk tubuh pada pertumbuhan.</t>
-  </si>
-  <si>
-    <t>karena bumi berputar pada porosnya.</t>
-  </si>
-  <si>
-    <t>perubahan benda padat menjadi uap.</t>
-  </si>
-  <si>
-    <t>kayu akan menyerap air.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Karena bumi berotasi </t>
   </si>
   <si>
     <t>Benda padat ke gas</t>
   </si>
   <si>
-    <t>pertumbuhan suatu makhluk hidup hewan yang memengaruhi bentuk fisiknya</t>
-  </si>
-  <si>
     <t>karena rotasi bumi</t>
   </si>
   <si>
-    <t>perubahan wujud partikel padat menjadi gas</t>
-  </si>
-  <si>
     <t>massa jenis air lebih besar daripada massa jenis kayu</t>
   </si>
   <si>
@@ -354,30 +249,18 @@
     <t>berubahnya benda dari padat menjadi gas</t>
   </si>
   <si>
-    <t>karena massa jenis air lebih besar daripada kayu, dan kerapatan air juga lebih rapat daripada kayu</t>
-  </si>
-  <si>
     <t>Karena bumi berotasi ketika mengelilingi matahari</t>
   </si>
   <si>
-    <t>Proses perubahan wujud dari padat menjadi gas</t>
-  </si>
-  <si>
     <t>Karena massa air lebih besar daripada kayu</t>
   </si>
   <si>
     <t>Karena adanya proses pemuaian jika terkena panas di siang hari</t>
   </si>
   <si>
-    <t>Perubahan bentuk tubuh pada hewan</t>
-  </si>
-  <si>
     <t>Karena pergerakan rotasi bumi pada porosnya</t>
   </si>
   <si>
-    <t>Perubahan wujud zat padat menjadi gas</t>
-  </si>
-  <si>
     <t>Karena massa jenis kayu lebih kecil dibandingkan massa jenis air</t>
   </si>
   <si>
@@ -390,42 +273,15 @@
     <t>rotasi bumi</t>
   </si>
   <si>
-    <t>perubahan wujud dari padat menjadi gas</t>
-  </si>
-  <si>
     <t>kayu memiliki massa jenis lebih ringan daripada air</t>
   </si>
   <si>
-    <t>agar relnya tidak membengkok ketika terjadi penambahan zat</t>
-  </si>
-  <si>
-    <t>karena massa kayu lebih ringan dibandingkan massa air.</t>
-  </si>
-  <si>
-    <t>memudahkan terjadinya pemuaian.</t>
-  </si>
-  <si>
-    <t>proses perkembangan biologi pada hewan berupa perubahan bentuk dari lahir hingga dewasa.</t>
-  </si>
-  <si>
-    <t>karena bumi berputar, sehingga bagian yang terkena sinar matahari disebut siang dan bagain yang tidak terkena sinar matahari disebut malam.</t>
-  </si>
-  <si>
-    <t>perubahan wujud padat menjadi gas.</t>
-  </si>
-  <si>
-    <t>massa jenis kayu lebih kecil daripada massa jenis air.</t>
-  </si>
-  <si>
     <t>Untuk menghindari pemuaian di siang hari</t>
   </si>
   <si>
     <t xml:space="preserve">Perkembangan hewan yang menyebabkan berubahnya fisik </t>
   </si>
   <si>
-    <t>Karena bumi berotasi mengelilingi matahari. Bagian bumi yang terkena cahaya matahari akan mengalami siang, sedangkan bagian bumi yang tidak terkena cahaya akan mengalami malam</t>
-  </si>
-  <si>
     <t>Perubahan wujud dari bentuk padat menjadi gas</t>
   </si>
   <si>
@@ -438,21 +294,9 @@
     <t>perubahan fisik pada hewan saat mengalami masa pertumbuhan</t>
   </si>
   <si>
-    <t>karena adanya rotasi bumi,yaitu bumi berputar pada porosnya</t>
-  </si>
-  <si>
-    <t>perubahan wujud benda dari padat menjadi gas</t>
-  </si>
-  <si>
     <t>karena gaya apung kayu lebih besar daripada gaya gravitasi</t>
   </si>
   <si>
-    <t>Karena pada rel kereta api dapat terjadi pemuaian, maka hal itu dibuat agar saat memuai rel kereta tidak melengkung keatas dan membahayakan kereta yang melintas</t>
-  </si>
-  <si>
-    <t>Karena adanya rotasi bumi dari pusatnya, daerah yang terpapar sinar matahari menjadi siang, dan yang tidak terkena cahaya matahari adalah malam</t>
-  </si>
-  <si>
     <t>Karena adanya perbedaan massa jenis</t>
   </si>
   <si>
@@ -477,63 +321,30 @@
     <t xml:space="preserve">Perubahan bentuk dari padat ke gas </t>
   </si>
   <si>
-    <t>karena rel kereta mengalami pemuaian yang bisa bikin rel melengkung dan membahayakan perjalanan kereta</t>
-  </si>
-  <si>
-    <t>untuk mengantisipasi jika rel memuai pada siang hari</t>
-  </si>
-  <si>
-    <t>karena saat panas siang hari besi pada rel akan memuai. ruang yang renggang diperlukan saat besi tersebut memuai</t>
-  </si>
-  <si>
-    <t>karena jika tidak dibuat renggang akan mengakibatkan tidak adanya ruang untuk pemuaian</t>
-  </si>
-  <si>
     <t>agar ketika rel mengalami pemuaian tidak menimbulkan bahaya untuk kereta yang berjalan</t>
   </si>
   <si>
-    <t>gunanya untuk memberi ruang ketika melar saat panas.</t>
-  </si>
-  <si>
     <t>Karena rel kereta yg terkena panas matahari nanti akan memuai dan memanjang</t>
   </si>
   <si>
-    <t>Dibuat renggang agar ketika suhu meningkat (krn panas) dan terjadi pemuaian, relnya tidak melengkung keatas</t>
-  </si>
-  <si>
     <t>untuk mencegah pemuaian pada siang hari</t>
   </si>
   <si>
     <t>agar pada saat panas masih ada ruang untuk memuai</t>
   </si>
   <si>
-    <t xml:space="preserve">untuk mengantisipasi pemuaian yang dapat terjadi. </t>
-  </si>
-  <si>
     <t xml:space="preserve"> proses perubahan serangga dari telur hingga dewasa</t>
   </si>
   <si>
-    <t xml:space="preserve"> perubahan bentuk yang terjadi pada kupu kupu dimana tadinya seekor ulat menjadi kupu-kupu.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> perubahan bentuk makhluk hidup di masa pertumbuhannya</t>
   </si>
   <si>
     <t xml:space="preserve"> proses perkembangan hewan yang melibatkan perubahan bentuk fisik</t>
   </si>
   <si>
-    <t xml:space="preserve"> siklus pembentukan hewan dari telur hingga menjadi bentuk yg sempurna</t>
-  </si>
-  <si>
     <t>Perubahan bentuk mahluk hidup yang terdapat fase kepompong</t>
   </si>
   <si>
-    <t>Perubahan pada hewan untuk mencapai kedewasaan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suatu proses perkembangan biologi pada hewan yang melibatkan perubahan penampilan fisik dan/atau struktur setelah kelahiran atau penetasan. </t>
-  </si>
-  <si>
     <t>perubahan dari telur sampai kupu-kupu</t>
   </si>
   <si>
@@ -543,12 +354,6 @@
     <t xml:space="preserve">  suatu keadaan yang tidak ada oksigen yang lama kelamaan akan habis</t>
   </si>
   <si>
-    <t xml:space="preserve">  perubahan wujud dari padat menjadi gas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  perubahan wujud dari padat ke gas </t>
-  </si>
-  <si>
     <t>kondisi di mana zat benda padat berubah menjadi gas</t>
   </si>
   <si>
@@ -585,9 +390,6 @@
     <t xml:space="preserve">massa jenis kayu lebih ringan/kecil dari massa jenis air </t>
   </si>
   <si>
-    <t xml:space="preserve">semakin kecil massa jenisnya dibandingkan dengan air, benda itu akan mengapung diatasnya. </t>
-  </si>
-  <si>
     <t>Karena akan menyerap air sehingga kayu akan mengembang Karena bermuatan air</t>
   </si>
   <si>
@@ -609,16 +411,226 @@
     <t>Karna adanya rotasi bumi</t>
   </si>
   <si>
-    <t>Karena pada siang hari sinar matahari menyebabkan besi rel kereta memuai  menyebabkan rel bengkok.</t>
-  </si>
-  <si>
-    <t>agar ketika rel memuai tidak bertabrakkan dengan rel di sekitarnya.</t>
-  </si>
-  <si>
     <t>karena bumi memutari matahari</t>
   </si>
   <si>
     <t>bumi berputar pada porosnya</t>
+  </si>
+  <si>
+    <t>perubahan wujud hidup suatu mahluk hidup dari telur  ulat  pupa  hingga kupu-kupu dewasa</t>
+  </si>
+  <si>
+    <t>karena massa jenis air lebih besar daripada kayu  dan kerapatan air juga lebih rapat daripada kayu</t>
+  </si>
+  <si>
+    <t>Dibuat renggang agar ketika suhu meningkat (krn panas) dan terjadi pemuaian  relnya tidak melengkung keatas</t>
+  </si>
+  <si>
+    <t>Karena pada rel kereta api dapat terjadi pemuaian  maka hal itu dibuat agar saat memuai rel kereta tidak melengkung keatas dan membahayakan kereta yang melintas</t>
+  </si>
+  <si>
+    <t>karena saat panas siang hari besi pada rel akan memuai  ruang yang renggang diperlukan saat besi tersebut memuai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perubahan wujud dari padat menjadi gas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">semakin kecil massa jenisnya dibandingkan dengan air  benda itu akan mengapung diatasnya  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menghindari pemuaian pada siang hari </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adanya rotasi bumi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perubahan dari zat padat ke gas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karena kayu memiliki serat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gunanya untuk memberi ruang ketika melar saat panas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">karena bumi berputar pada porosnya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kayu akan menyerap air </t>
+  </si>
+  <si>
+    <t xml:space="preserve">agar ketika rel memuai tidak bertabrakkan dengan rel di sekitarnya </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> perubahan bentuk yang terjadi pada kupu kupu dimana tadinya seekor ulat menjadi kupu-kupu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">karena massa kayu lebih ringan dibandingkan massa air </t>
+  </si>
+  <si>
+    <t xml:space="preserve">memudahkan terjadinya pemuaian </t>
+  </si>
+  <si>
+    <t xml:space="preserve">proses perkembangan biologi pada hewan berupa perubahan bentuk dari lahir hingga dewasa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">massa jenis kayu lebih kecil daripada massa jenis air </t>
+  </si>
+  <si>
+    <t xml:space="preserve">untuk mengantisipasi pemuaian yang dapat terjadi  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karena mencegah pemuaian saat siang hari </t>
+  </si>
+  <si>
+    <t xml:space="preserve">karena rel kereta memuai yang bisa bikin rel melengkung </t>
+  </si>
+  <si>
+    <t>Untuk mengantisipasi jika rel memuai pada siang hari</t>
+  </si>
+  <si>
+    <t>Karena sinar matahari menyebabkan rel kereta memuai  dan melengkung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">karena efeknya akan membuat rel melengkung </t>
+  </si>
+  <si>
+    <t>Karena jika pemuaian terjadi maka rel tidak melengkung</t>
+  </si>
+  <si>
+    <t>Agar saat terjadi pemuaian rel tidak melengkung</t>
+  </si>
+  <si>
+    <t>agar relnya tidak melengkung ketika terjadi penambahan zat</t>
+  </si>
+  <si>
+    <t>Suatu proses perkembangan tubuh binatang</t>
+  </si>
+  <si>
+    <t>Intinya suatu perkembangan dari tubuh mahluk hidup untuk lebih sempurna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perubahan bentuk biologis dalam masa perkembangan hewan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perkembangan biologi pada hewan dan perubahan fisik </t>
+  </si>
+  <si>
+    <t>Proses perubahan wujud dari larva sampai jadi kupu kupu</t>
+  </si>
+  <si>
+    <t>Perkembangan tubuh fauna</t>
+  </si>
+  <si>
+    <t>perkembangan biologi pada binatang</t>
+  </si>
+  <si>
+    <t>Perkembangan biologi pada fisik</t>
+  </si>
+  <si>
+    <t>Perubahan atau berkembang fauna</t>
+  </si>
+  <si>
+    <t>Perubahan tubuh pada binatang untuk mencapai kedewasaan</t>
+  </si>
+  <si>
+    <t>Proses perkembangan wujud pada fauna</t>
+  </si>
+  <si>
+    <t>perubahan bentuk tubuh pada binatang</t>
+  </si>
+  <si>
+    <t>pertumbuhan suatu hewan yang memengaruhi bentuk fisiknya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> siklus pembentukan binatang dari telur hingga menjadi bentuk yg sempurna</t>
+  </si>
+  <si>
+    <t>Perubahan bentuk tubuh pada fauna</t>
+  </si>
+  <si>
+    <t>Karena matahari dan bumi melakukan rotasi</t>
+  </si>
+  <si>
+    <t>perputaran bumi</t>
+  </si>
+  <si>
+    <t>Karena bumi berputar pada porosnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karena bumi berputar pada porosnya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">karena bumi berotasi (berputar) </t>
+  </si>
+  <si>
+    <t>Karena bumi melakukan rotasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">karena bumi berputar </t>
+  </si>
+  <si>
+    <t>karena adanya rotasi bumi pada porosnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karena adanya rotasi bumi dari pusatnya </t>
+  </si>
+  <si>
+    <t>Pergantian wujud dari padat menjadi gas</t>
+  </si>
+  <si>
+    <t>Pergantian wujud padat ke wujud gas</t>
+  </si>
+  <si>
+    <t>Pergantian wujud pada benda padat menjadi gas</t>
+  </si>
+  <si>
+    <t>Zat padat berganti menjadi gas</t>
+  </si>
+  <si>
+    <t>Pergantian bentuk dari padat menjadi gas</t>
+  </si>
+  <si>
+    <t>perubahan bentuk benda padat menjadi gas</t>
+  </si>
+  <si>
+    <t>perubahan bentuk dari benda padat menjadi gas</t>
+  </si>
+  <si>
+    <t>pergantian bentuk benda padat menjadi gas</t>
+  </si>
+  <si>
+    <t>Perubahan bentuk  dari padat menjadi gas</t>
+  </si>
+  <si>
+    <t>Pergantian wujud jenis benda dari padat ke uap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perubahan bentuk benda padat menjadi uap </t>
+  </si>
+  <si>
+    <t>pergantian wujud padat menjadi gas</t>
+  </si>
+  <si>
+    <t>Proses pergantian wujud dari padat menjadi gas</t>
+  </si>
+  <si>
+    <t>perubahan bentuk dari padat menjadi gas</t>
+  </si>
+  <si>
+    <t>Perubahan bentuk zat padat menjadi gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perubahan bentuk padat menjadi gas </t>
+  </si>
+  <si>
+    <t>pergantian wujud benda dari padat menjadi gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pergantian bentuk dari padat menjadi gas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  pergantian bentuk dari padat ke gas </t>
   </si>
 </sst>
 </file>
@@ -910,8 +922,8 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -950,13 +962,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -964,19 +976,19 @@
         <v>44211.729263182875</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -984,19 +996,19 @@
         <v>44211.733176018519</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>183</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1004,19 +1016,19 @@
         <v>44211.740133518513</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>178</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1024,19 +1036,19 @@
         <v>44211.742248969909</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>161</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>186</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1044,19 +1056,19 @@
         <v>44211.743494722221</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>159</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1064,19 +1076,19 @@
         <v>44211.748136909722</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
+        <v>185</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>179</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1084,19 +1096,19 @@
         <v>44211.759312870374</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>180</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1104,19 +1116,19 @@
         <v>44211.790664895831</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>179</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>181</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1124,19 +1136,19 @@
         <v>44211.791498599538</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>195</v>
+        <v>129</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>184</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1144,19 +1156,19 @@
         <v>44211.795686550926</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>185</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1164,19 +1176,19 @@
         <v>44211.797738483801</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>47</v>
+        <v>188</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1184,19 +1196,19 @@
         <v>44211.79911521991</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>190</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1204,19 +1216,19 @@
         <v>44211.8075068287</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>199</v>
+        <v>131</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1224,19 +1236,19 @@
         <v>44211.813821620366</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>173</v>
+        <v>110</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1244,19 +1256,19 @@
         <v>44211.814990717598</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>60</v>
+        <v>191</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1264,19 +1276,19 @@
         <v>44211.815106817128</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>192</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1284,19 +1296,19 @@
         <v>44211.815677303239</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1304,19 +1316,19 @@
         <v>44211.816781724541</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>176</v>
+        <v>111</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>186</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1324,19 +1336,19 @@
         <v>44211.817908206023</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>165</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1344,19 +1356,19 @@
         <v>44211.819407743053</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1364,19 +1376,19 @@
         <v>44211.821221678241</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>171</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1384,19 +1396,19 @@
         <v>44211.821241712962</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1404,19 +1416,19 @@
         <v>44211.823395486106</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>91</v>
+        <v>194</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1424,19 +1436,19 @@
         <v>44211.824329560186</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>95</v>
+        <v>195</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1444,19 +1456,19 @@
         <v>44211.824706666666</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>168</v>
+        <v>107</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>189</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1464,19 +1476,19 @@
         <v>44211.825924745368</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1484,19 +1496,19 @@
         <v>44211.827162384259</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1504,19 +1516,19 @@
         <v>44211.829924432866</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1524,19 +1536,19 @@
         <v>44211.83350518519</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>163</v>
+        <v>104</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>113</v>
+        <v>197</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1544,19 +1556,19 @@
         <v>44211.842798379628</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1564,19 +1576,19 @@
         <v>44211.85447387732</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1584,19 +1596,19 @@
         <v>44211.871311608797</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>198</v>
+        <v>130</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>177</v>
+        <v>112</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1604,19 +1616,19 @@
         <v>44211.871355393523</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1624,19 +1636,19 @@
         <v>44211.872718333332</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1644,19 +1656,19 @@
         <v>44211.874140636573</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1664,19 +1676,19 @@
         <v>44211.87667636574</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1684,19 +1696,19 @@
         <v>44211.879279502318</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1704,19 +1716,19 @@
         <v>44211.888182187497</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>148</v>
+        <v>96</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1724,19 +1736,19 @@
         <v>44211.904157002311</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>185</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1744,41 +1756,41 @@
         <v>44211.944198275465</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>187</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>192</v>
+        <v>126</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>193</v>
+        <v>127</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>194</v>
+        <v>128</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>